<commit_message>
Tue Dec 31 10:41:09 AM EST 2024
</commit_message>
<xml_diff>
--- a/iron_oxo_DDCASPT2/iron_VDZP_params.xlsx
+++ b/iron_oxo_DDCASPT2/iron_VDZP_params.xlsx
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6">
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.001</v>
+        <v>1e-06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wed Jan 15 02:07:37 PM EST 2025 best iron
</commit_message>
<xml_diff>
--- a/iron_oxo_DDCASPT2/iron_VDZP_params.xlsx
+++ b/iron_oxo_DDCASPT2/iron_VDZP_params.xlsx
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5">
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="7">

</xml_diff>